<commit_message>
hey i did some stuff
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\Super Points repo\SMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnq\Documents\GitHub\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6CF912-4B0C-4699-891E-9DA3737114EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4604A72-55E1-49D7-BE1F-E8510166ADBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
   </bookViews>
@@ -378,23 +378,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9DE083-53AB-458A-AE28-C97092FEF2EB}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,15 +728,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
@@ -750,14 +750,14 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -906,14 +906,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -998,10 +998,10 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1032,10 +1032,10 @@
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>43</v>
       </c>
       <c r="D21" s="16" t="s">
@@ -1053,7 +1053,7 @@
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="16" t="s">
@@ -1066,12 +1066,12 @@
         <v>48</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="24"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1080,7 +1080,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="24"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1089,7 +1089,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="24"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1098,20 +1098,20 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>

</xml_diff>

<commit_message>
risk & test cases
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\Super Points repo\SMP2\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B39406-FBF3-49C9-A92E-3D99AF4E50A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8A7B95-ADF9-48C1-87F3-74B88EE9129B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="2" r:id="rId1"/>
     <sheet name="Iteration 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Iteration 3" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="138">
   <si>
     <t>Input</t>
   </si>
@@ -514,6 +515,55 @@
   </si>
   <si>
     <t>User should be redirected to log in page</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Date of testing: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2019-05-16</t>
+    </r>
+  </si>
+  <si>
+    <t>Attempt to log into a user that does not exist</t>
+  </si>
+  <si>
+    <t>Username: [aaaaaaaaaaaaaaaaaaa], Password: [aaaaaaaaaaa]</t>
+  </si>
+  <si>
+    <t>Toast with exception message</t>
+  </si>
+  <si>
+    <t>Attempt to enter a SQL statement via the login page</t>
+  </si>
+  <si>
+    <t>Username: [dmr], Password: [' OR 'A'='A]</t>
+  </si>
+  <si>
+    <t>Logout of new Business. Username: [1], Password: [1]</t>
+  </si>
+  <si>
+    <t>Logout out of the business and enter into the newly created user. Username: [Username from step 2], Password: [Password from step 3]</t>
+  </si>
+  <si>
+    <t>Change user notification settings</t>
+  </si>
+  <si>
+    <t>Move "slider" to the leftmost, re-open application</t>
+  </si>
+  <si>
+    <t>User should have no notification upon logging in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User has no notification when logging in </t>
   </si>
 </sst>
 </file>
@@ -610,7 +660,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -693,6 +743,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1011,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF9DE083-53AB-458A-AE28-C97092FEF2EB}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection sqref="A1:G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,15 +1080,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
@@ -1049,14 +1102,14 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1205,14 +1258,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1297,10 +1350,10 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="31"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1440,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F024C0B-2EBF-4B53-977C-D029A13E0302}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -1457,15 +1510,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="27"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
@@ -1479,14 +1532,14 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1801,11 +1854,11 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
@@ -2035,11 +2088,11 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
@@ -2133,11 +2186,11 @@
       <c r="G36" s="30"/>
     </row>
     <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
@@ -2264,4 +2317,894 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FBA6B7-06CC-41CB-A0E9-373FC7E0E078}">
+  <dimension ref="A1:H47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="31"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>5</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>6</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>7</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>8</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>9</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>11</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>12</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>13</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>13</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>14</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>15</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>16</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>1</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>3</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>4</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>5</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>6</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>7</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>8</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>9</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="30"/>
+    </row>
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="30">
+        <v>1</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F43" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="30"/>
+    </row>
+    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="30">
+        <v>2</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="30"/>
+    </row>
+    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="30">
+        <v>3</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="30"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C37" r:id="rId1" display="http://ec2-99-79-49-31.ca-central-1.compute.amazonaws.com/scripts.php?function=sendEmail" xr:uid="{2F25AE8E-1DAE-4572-A719-B3D17924E411}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
php changes & test case
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\Super Points repo\SMP2\SMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8A7B95-ADF9-48C1-87F3-74B88EE9129B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31013E5D-8166-4210-A785-8D42A149C93F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{6446E0C1-1C89-49C9-B74C-64B6F8926156}"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="2" r:id="rId1"/>
     <sheet name="Iteration 2" sheetId="4" r:id="rId2"/>
     <sheet name="Iteration 3" sheetId="6" r:id="rId3"/>
+    <sheet name="Iteration 4" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="156">
   <si>
     <t>Input</t>
   </si>
@@ -564,6 +565,60 @@
   </si>
   <si>
     <t xml:space="preserve">User has no notification when logging in </t>
+  </si>
+  <si>
+    <t>Scenario: #4, Additional Graph Testing</t>
+  </si>
+  <si>
+    <t>Username: [1], Password: [1]</t>
+  </si>
+  <si>
+    <t>Artificially create "visits" with users who have not entered the store before</t>
+  </si>
+  <si>
+    <t>Create new rows inside the visit table and create new rows in the points table</t>
+  </si>
+  <si>
+    <t>Check pie chart to see if the new users matches the number of rows created</t>
+  </si>
+  <si>
+    <t>New users have increased by the number of rows entered</t>
+  </si>
+  <si>
+    <t>Check line chart to see if the number of visits have increased</t>
+  </si>
+  <si>
+    <t>Chart handles the increase in visits</t>
+  </si>
+  <si>
+    <t>Check bar chart to see if the graph has increased</t>
+  </si>
+  <si>
+    <t>Users increase based on the users created</t>
+  </si>
+  <si>
+    <t>Enter special characters in the search filter</t>
+  </si>
+  <si>
+    <t>Use ", %, '</t>
+  </si>
+  <si>
+    <t>Filters properly</t>
+  </si>
+  <si>
+    <t>Confirm the tables have correct information</t>
+  </si>
+  <si>
+    <t>Information is confirmed and correct</t>
+  </si>
+  <si>
+    <t>Create a new business and confirm the above steps have adjusted for the new business</t>
+  </si>
+  <si>
+    <t>Sign-up as a new business user (tested in regression testing)</t>
+  </si>
+  <si>
+    <t>All steps adjust to new business</t>
   </si>
 </sst>
 </file>
@@ -660,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -746,6 +801,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1080,15 +1141,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
@@ -1102,14 +1163,14 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1258,14 +1319,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1350,10 +1411,10 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="31"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1510,15 +1571,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
@@ -1532,14 +1593,14 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1854,11 +1915,11 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
@@ -1998,7 +2059,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="144" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
         <v>6</v>
       </c>
@@ -2088,11 +2149,11 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="26"/>
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
@@ -2186,11 +2247,11 @@
       <c r="G36" s="30"/>
     </row>
     <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
@@ -2321,9 +2382,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FBA6B7-06CC-41CB-A0E9-373FC7E0E078}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2340,15 +2401,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="31"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
@@ -2362,14 +2423,14 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2744,11 +2805,11 @@
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
@@ -2884,9 +2945,7 @@
       <c r="F29" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="19" t="s">
-        <v>94</v>
-      </c>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
@@ -2907,9 +2966,7 @@
       <c r="F30" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="28" t="s">
-        <v>95</v>
-      </c>
+      <c r="G30" s="28"/>
       <c r="H30" s="20" t="s">
         <v>116</v>
       </c>
@@ -2978,11 +3035,11 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
@@ -3037,163 +3094,247 @@
       <c r="A38">
         <v>2</v>
       </c>
-      <c r="B38" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="30" t="s">
-        <v>101</v>
+      <c r="B38" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>7</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="F38" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="30"/>
+        <v>152</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
       <c r="B39" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C40" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D40" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E40" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="F39" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G39" s="30"/>
-    </row>
-    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
+      <c r="F40" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D45" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G45" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="H45" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="30">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="30">
         <v>1</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B46" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="30" t="s">
+      <c r="C46" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E46" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="F43" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="30"/>
-    </row>
-    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="30">
+      <c r="F46" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="30">
         <v>2</v>
       </c>
-      <c r="B44" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="F44" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="30"/>
-    </row>
-    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="30">
+      <c r="B47" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="30">
         <v>3</v>
       </c>
-      <c r="B45" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="F45" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="30"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
+      <c r="B48" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="30">
+        <v>4</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="30"/>
+    </row>
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="30">
+        <v>5</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A1:C1"/>
@@ -3207,4 +3348,974 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F0F6CB-D78F-4B9E-976D-D2F072261A86}">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="36.5546875" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>5</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>6</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>7</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>8</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>9</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>11</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>12</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>13</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>13</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>14</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>15</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>16</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>1</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" ht="144" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
+        <v>3</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>4</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>5</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>6</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>7</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>8</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>9</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="30">
+        <v>1</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="30">
+        <v>2</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="30">
+        <v>3</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="30"/>
+    </row>
+    <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="30">
+        <v>4</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="30"/>
+    </row>
+    <row r="50" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="30">
+        <v>5</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A35:C35"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C37" r:id="rId1" display="http://ec2-99-79-49-31.ca-central-1.compute.amazonaws.com/scripts.php?function=sendEmail" xr:uid="{2DDFFFA4-9C73-4271-ABCA-B6D9B64313CA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>